<commit_message>
now includes the latest plant that still started flowering
</commit_message>
<xml_diff>
--- a/doc/histogram flowering time Brassica F1.xlsx
+++ b/doc/histogram flowering time Brassica F1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="27729"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1660" yWindow="1540" windowWidth="39140" windowHeight="24660"/>
+    <workbookView xWindow="980" yWindow="1560" windowWidth="31380" windowHeight="22200"/>
   </bookViews>
   <sheets>
     <sheet name="Grafiek1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>11/12/2017 to 20/12/2017</t>
   </si>
@@ -226,6 +226,50 @@
   </si>
   <si>
     <t>176-239</t>
+  </si>
+  <si>
+    <t>17208**</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">17102, 17109, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>17112**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, 17118, 17120, 17121, 17122, 17127, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>17130**</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 17208**</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -318,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
@@ -372,16 +416,25 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -808,6 +861,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-3ED6-2A4A-A3BA-C367B1026FA9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -828,11 +886,25 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-3ED6-2A4A-A3BA-C367B1026FA9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000020-BDF5-8C4D-A1E7-8A133957FBA5}"/>
@@ -843,6 +915,15 @@
             <c:idx val="16"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000F-A03A-2B4B-B017-82E3E7E2B2CA}"/>
@@ -883,6 +964,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000025-3ED6-2A4A-A3BA-C367B1026FA9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="20"/>
@@ -897,13 +983,18 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000027-3ED6-2A4A-A3BA-C367B1026FA9}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$22</c:f>
+              <c:f>Sheet1!$B$2:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>113.0</c:v>
                 </c:pt>
@@ -966,16 +1057,19 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>328.0</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>456.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$22</c:f>
+              <c:f>Sheet1!$D$2:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -1037,6 +1131,9 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1058,11 +1155,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2065741688"/>
-        <c:axId val="-2065737992"/>
+        <c:axId val="-2014598136"/>
+        <c:axId val="-2014594648"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="-2065741688"/>
+        <c:axId val="-2014598136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1090,7 +1187,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1105,23 +1202,23 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065737992"/>
+        <c:crossAx val="-2014594648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="5.0"/>
+        <c:majorUnit val="10.0"/>
         <c:majorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2065737992"/>
+        <c:axId val="-2014594648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="11.0"/>
           <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="r"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1139,7 +1236,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -1167,8 +1264,8 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065741688"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="-2014598136"/>
+        <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -1215,7 +1312,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="228" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="201" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -1226,7 +1323,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9207500" cy="5614737"/>
+    <xdr:ext cx="9205369" cy="5616980"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafiek 1"/>
@@ -1546,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1922,139 +2019,140 @@
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="22">
+      <c r="A22" s="29">
         <v>43282</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B22" s="25">
         <v>328</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="27">
         <v>1</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="9"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="17"/>
+      <c r="A23" s="22">
+        <v>43380</v>
+      </c>
+      <c r="B23" s="23">
+        <v>456</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="23">
+        <v>1</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="9"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="17"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" s="9" customFormat="1">
-      <c r="A25" s="15" t="s">
+      <c r="B25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" s="9" customFormat="1">
+      <c r="A26" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="19" t="s">
+      <c r="B26" s="15"/>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B27" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C27" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D27" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E27" s="19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="61">
-      <c r="A27" s="4" t="s">
+    <row r="28" spans="1:7" ht="61">
+      <c r="A28" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C28" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D28" s="6">
         <v>11</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E28" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45">
-      <c r="A28" s="4" t="s">
+    <row r="29" spans="1:7" ht="45">
+      <c r="A29" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C29" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D29" s="6">
         <v>8</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E29" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="76">
-      <c r="A29" s="4" t="s">
+    <row r="30" spans="1:7" ht="76">
+      <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C30" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D30" s="6">
         <v>11</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="E30" s="12" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="4">
-        <v>43201</v>
-      </c>
-      <c r="B30" s="21">
-        <v>247</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="6">
-        <v>2</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="4">
-        <v>43234</v>
+        <v>43201</v>
       </c>
       <c r="B31" s="21">
-        <v>280</v>
-      </c>
-      <c r="C31" s="5">
-        <v>17111</v>
+        <v>247</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D31" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>11</v>
@@ -2062,13 +2160,13 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="4">
-        <v>43248</v>
+        <v>43234</v>
       </c>
       <c r="B32" s="21">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="C32" s="5">
-        <v>17101</v>
+        <v>17111</v>
       </c>
       <c r="D32" s="6">
         <v>1</v>
@@ -2077,49 +2175,49 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="77">
-      <c r="A33" s="6" t="s">
+    <row r="33" spans="1:5">
+      <c r="A33" s="4">
+        <v>43248</v>
+      </c>
+      <c r="B33" s="21">
+        <v>293</v>
+      </c>
+      <c r="C33" s="5">
+        <v>17101</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="77">
+      <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="21">
+      <c r="B34" s="21">
         <v>294</v>
       </c>
-      <c r="C33" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="6">
+      <c r="C34" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="6">
         <v>10</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E34" s="13" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="4">
-        <v>43269</v>
-      </c>
-      <c r="B34" s="21">
-        <v>315</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="6">
-        <v>1</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="4">
-        <v>43282</v>
+        <v>43269</v>
       </c>
       <c r="B35" s="21">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D35" s="6">
         <v>1</v>
@@ -2129,19 +2227,53 @@
       </c>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="4">
+        <v>43282</v>
+      </c>
+      <c r="B36" s="21">
+        <v>328</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" s="6">
+        <v>1</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="22">
+        <v>43380</v>
+      </c>
+      <c r="B37" s="23">
+        <v>456</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="23">
+        <v>1</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="17"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="18" t="s">
+      <c r="B38" s="17"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="18"/>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="18" t="s">
+      <c r="B39" s="18"/>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="18" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>